<commit_message>
Add tax calculation to Excel update and modify output structure
</commit_message>
<xml_diff>
--- a/contabilidad.xlsx
+++ b/contabilidad.xlsx
@@ -314,7 +314,7 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -338,16 +338,24 @@
           <t>cantidad</t>
         </is>
       </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>impuestos</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="n">
-        <v>100.5</v>
+        <v>10.43</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>1</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>